<commit_message>
changes made to page and testData
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/OpenCartTestData.xlsx
+++ b/src/test/resources/testData/OpenCartTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="6075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t xml:space="preserve">subscribe </t>
   </si>
   <si>
-    <t>Javad</t>
-  </si>
-  <si>
     <t>Adeli</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>Kasra018126</t>
   </si>
   <si>
-    <t>Azima</t>
-  </si>
-  <si>
     <t>Kazemian</t>
   </si>
   <si>
@@ -71,10 +65,16 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>m.jawadadeli12345@gmail.com</t>
-  </si>
-  <si>
-    <t>azimeh.kazemian145686@ucf.edu</t>
+    <t xml:space="preserve">Mohammad </t>
+  </si>
+  <si>
+    <t>Azimeh</t>
+  </si>
+  <si>
+    <t>m.jawadadeli123450012222@gmail.com</t>
+  </si>
+  <si>
+    <t>azimeh.kazemian14568633309909@ucf.edu</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,42 +455,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>